<commit_message>
added price data sheet
</commit_message>
<xml_diff>
--- a/price/pricedata.xlsx
+++ b/price/pricedata.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BTC" sheetId="1" r:id="rId1"/>
     <sheet name="ETH" sheetId="2" r:id="rId2"/>
     <sheet name="ETC" sheetId="3" r:id="rId3"/>
+    <sheet name="notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>coinmarketcap.com</t>
   </si>
 </sst>
 </file>
@@ -137,8 +141,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -415,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -92630,4 +92662,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>